<commit_message>
All 2VP Data Uploaded
</commit_message>
<xml_diff>
--- a/DragPrediction/Data/Drag Values.xlsx
+++ b/DragPrediction/Data/Drag Values.xlsx
@@ -285,15 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,6 +299,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2419,13 +2419,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:colOff>1257300</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
@@ -2746,7 +2746,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2766,26 +2766,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3170,22 +3170,22 @@
       <c r="C10" s="5">
         <v>2.7034464531040105E-2</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>4.0190154194527726E-2</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="20">
         <v>3.9950589297076929E-3</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>7.8922922486017472E-3</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>5.5611285058155364E-4</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="22">
         <v>4.9416722388687148E-2</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="22">
         <v>9.5501389213822341E-2</v>
       </c>
       <c r="J10" s="5"/>
@@ -3204,22 +3204,22 @@
       <c r="C11" s="5">
         <v>2.3191202074720297E-2</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <v>1.7723549021326026E-2</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>2.2066433306492891E-3</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>8.9959710507998489E-3</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>5.4008440610467672E-4</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="22">
         <v>0.11189019580904892</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="22">
         <v>8.1923580203644208E-2</v>
       </c>
       <c r="J11" s="5"/>
@@ -3231,29 +3231,29 @@
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="20">
         <f>27.59814224/(0.5*1.227634*13.4112^2*1.151455)</f>
         <v>0.21709943244099184</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>2.0505898102416559E-2</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>1.3538516874291971E-2</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>1.8338616595283826E-3</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>8.3935110377911706E-3</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>5.4411305163339129E-4</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="22">
         <v>8.1852782145029349E-2</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="22">
         <v>0.13524663267511233</v>
       </c>
       <c r="J12" s="5"/>
@@ -3265,29 +3265,29 @@
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="20">
         <f>22.2952264/(0.5*1.227634*13.4112^2*1.151455)</f>
         <v>0.17538430505543395</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>2.7403389748523879E-2</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="20">
         <v>4.2215639452793295E-2</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="20">
         <v>4.1258268771948289E-3</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>8.0130029385400928E-3</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>5.6440566318064172E-4</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="20">
         <v>5.0480187893592009E-2</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="20">
         <v>0.12490413761461443</v>
       </c>
       <c r="J13" s="5"/>
@@ -3299,29 +3299,29 @@
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="20">
         <f>25.46586164/(0.5*1.227634*13.4112^2*1.151455)</f>
         <v>0.2003259516740872</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="20">
         <v>2.3888112033734889E-2</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="20">
         <v>2.2106848771575732E-2</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="20">
         <v>2.4738973488243549E-3</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>9.0748951532535118E-3</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>5.2475536778240524E-4</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="20">
         <v>9.2383757370461936E-2</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="20">
         <v>0.10794218140264572</v>
       </c>
       <c r="J14" s="5"/>
@@ -3333,29 +3333,29 @@
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="20">
         <f>27.02328633/(0.5*1.227634*13.4112^2*1.151455)</f>
         <v>0.21257735661751603</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="20">
         <v>2.0863746966304633E-2</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="20">
         <v>1.6396109808295263E-2</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="20">
         <v>1.9303782929027419E-3</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="20">
         <v>8.9394899329271003E-3</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>5.3562302710880624E-4</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="20">
         <v>7.1612362152152179E-2</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="20">
         <v>0.14096499186943504</v>
       </c>
       <c r="J15" s="5"/>
@@ -3367,28 +3367,28 @@
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="20">
         <v>0.19876012957652647</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="24">
         <v>2.7481962863308795E-2</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="24">
         <v>4.420000677190554E-2</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="24">
         <v>4.2670855236784976E-3</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="24">
         <v>7.1455670315535551E-3</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="24">
         <v>5.4654748221111835E-4</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="22">
         <v>0.13859538084759548</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="22">
         <v>6.0164693663774298E-2</v>
       </c>
       <c r="J16" s="5"/>
@@ -3400,28 +3400,28 @@
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="20">
         <v>0.20793165857327361</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="24">
         <v>2.4640541396873814E-2</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="24">
         <v>2.4634075151374283E-2</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="24">
         <v>2.6654713889205117E-3</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="24">
         <v>8.8436057622097008E-3</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="24">
         <v>5.4693034237920566E-4</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="22">
         <v>0.16026902652489311</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="22">
         <v>4.766259035619045E-2</v>
       </c>
       <c r="J17" s="5"/>
@@ -3433,28 +3433,28 @@
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="20">
         <v>0.22758579041522728</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="24">
         <v>2.2081183703235682E-2</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="24">
         <v>1.944454834903607E-2</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="24">
         <v>2.1221411278218721E-3</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="24">
         <v>8.9358713654867864E-3</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="24">
         <v>5.7500248060058604E-4</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="22">
         <v>0.13402969271203233</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="22">
         <v>9.3556094556614539E-2</v>
       </c>
       <c r="J18" s="5"/>
@@ -3478,16 +3478,16 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21" t="s">
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -3634,8 +3634,8 @@
         <f>C7+E7+G7</f>
         <v>2.7629316024036281E-2</v>
       </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
@@ -3724,10 +3724,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>